<commit_message>
fixing up integration tests
</commit_message>
<xml_diff>
--- a/modules/lib-excel/integtests/src/test/resources/org/incode/platform/lib/excel/integtests/tests/toDoItems-updated.xlsx
+++ b/modules/lib-excel/integtests/src/test/resources/org/incode/platform/lib/excel/integtests/tests/toDoItems-updated.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\isisaddons\isis-module-excel\integtests\src\test\resources\org\isisaddons\module\excel\integtests\demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\incodehq\incode-platform\modules\lib-excel\integtests\src\test\resources\org\incode\platform\lib\excel\integtests\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,7 +34,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>TODO:L_0</t>
+          <t>exampleLibExcel.ExcelModuleDemoToDoItem:L_0</t>
         </r>
       </text>
     </comment>
@@ -48,7 +48,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>TODO:L_1</t>
+          <t>exampleLibExcel.ExcelModuleDemoToDoItem:L_1</t>
         </r>
       </text>
     </comment>
@@ -183,7 +183,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1027" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="1027" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -226,7 +232,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="2" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -247,6 +259,60 @@
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
           <a:headEnd/>
           <a:tailEnd/>
         </a:ln>
@@ -582,15 +648,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>